<commit_message>
Finishing touches! Almost there!
</commit_message>
<xml_diff>
--- a/content/source.xlsx
+++ b/content/source.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="377">
   <si>
     <t>抢</t>
   </si>
@@ -2587,9 +2587,9 @@
   </sheetPr>
   <dimension ref="A1:H131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A107" zoomScale="179" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="179" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A131" sqref="A131"/>
+      <selection pane="topRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3112,7 +3112,9 @@
         <v>76</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="C25" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="3" t="s">
         <v>77</v>
@@ -3130,7 +3132,9 @@
         <v>79</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="C26" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="3" t="s">
         <v>80</v>
@@ -3170,7 +3174,9 @@
         <v>84</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="C28" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="3" t="s">
         <v>85</v>

</xml_diff>